<commit_message>
use dactyl manuform 6x7
</commit_message>
<xml_diff>
--- a/kbd_layout.xlsx
+++ b/kbd_layout.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradyumna\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8951D066-6D81-4FC8-A2E1-18C4EE8A639E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9617BE86-39A4-4F84-B105-3A622FD9B470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{335468D2-36C8-4DD8-8A44-AE5A18BFA141}"/>
+    <workbookView xWindow="2580" yWindow="7545" windowWidth="25245" windowHeight="16545" xr2:uid="{335468D2-36C8-4DD8-8A44-AE5A18BFA141}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="manuform 6x7" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="182">
   <si>
     <t>* 8</t>
   </si>
@@ -657,7 +658,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -839,11 +840,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -962,6 +976,39 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,6 +1034,203 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Circle: Hollow 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC1153CA-A70C-4E4D-A19B-DDD3616D4031}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5953125" y="838200"/>
+          <a:ext cx="209550" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="donut">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Circle: Hollow 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{298B6304-F11F-4850-B526-4EB0C3585A3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5953125" y="1628775"/>
+          <a:ext cx="209550" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="donut">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Circle: Hollow 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE5D5E3D-ACF2-4D6B-A07E-DA4B79DAAD50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="1228725"/>
+          <a:ext cx="209550" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="donut">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6221,10 +6465,1837 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC6952D-12D4-41C7-BA70-FE890F76783D}">
+  <dimension ref="A2:AK38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1">
+        <v>12</v>
+      </c>
+      <c r="S2" s="1">
+        <v>13</v>
+      </c>
+      <c r="T2" s="1">
+        <v>14</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>12</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE3" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V5" s="1">
+        <v>2</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" s="1">
+        <v>3</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD6" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="1">
+        <v>4</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="1">
+        <v>5</v>
+      </c>
+      <c r="W8" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="X8" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y8" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z8" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH8" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI8" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ8" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9"/>
+      <c r="M9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1">
+        <v>6</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V11" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>11</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>12</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P12" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q12" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="S12" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="T12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+      <c r="W12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="X12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA12" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB12" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE12" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF12" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ12" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="23">
+        <v>7</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>8</v>
+      </c>
+      <c r="R13" s="45">
+        <v>9</v>
+      </c>
+      <c r="S13" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="T13" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13" s="1">
+        <v>1</v>
+      </c>
+      <c r="W13" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="X13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF13" s="23">
+        <v>7</v>
+      </c>
+      <c r="AG13" s="24">
+        <v>8</v>
+      </c>
+      <c r="AH13" s="45">
+        <v>9</v>
+      </c>
+      <c r="AI13" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ13" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="26">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="27">
+        <v>5</v>
+      </c>
+      <c r="R14" s="27">
+        <v>6</v>
+      </c>
+      <c r="S14" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="T14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="V14" s="1">
+        <v>2</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF14" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="27">
+        <v>5</v>
+      </c>
+      <c r="AH14" s="27">
+        <v>6</v>
+      </c>
+      <c r="AI14" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>2</v>
+      </c>
+      <c r="R15" s="27">
+        <v>3</v>
+      </c>
+      <c r="S15" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V15" s="1">
+        <v>3</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC15" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD15" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF15" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="27">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="27">
+        <v>3</v>
+      </c>
+      <c r="AI15" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="O16" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="P16" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q16" s="49">
+        <v>0</v>
+      </c>
+      <c r="R16" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="S16" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" s="1">
+        <v>4</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="X16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF16" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG16" s="49">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI16" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="Q17" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="R17" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="S17" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="V17" s="1">
+        <v>5</v>
+      </c>
+      <c r="W17" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="X17" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y17" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z17" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH17" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI17" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ17" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="V18" s="1">
+        <v>6</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+    </row>
+    <row r="22" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+    </row>
+    <row r="23" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="AC23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+    </row>
+    <row r="24" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+    </row>
+    <row r="25" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+    </row>
+    <row r="26" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
+      <c r="AJ26"/>
+    </row>
+    <row r="27" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+    </row>
+    <row r="28" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+    </row>
+    <row r="29" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="AF29"/>
+      <c r="AG29"/>
+      <c r="AH29"/>
+      <c r="AI29"/>
+      <c r="AJ29"/>
+      <c r="AK29"/>
+    </row>
+    <row r="30" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="AF30"/>
+      <c r="AG30"/>
+      <c r="AH30"/>
+      <c r="AI30"/>
+      <c r="AJ30"/>
+      <c r="AK30"/>
+    </row>
+    <row r="31" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
+      <c r="AH31"/>
+      <c r="AI31"/>
+      <c r="AJ31"/>
+      <c r="AK31"/>
+    </row>
+    <row r="32" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+    </row>
+    <row r="33" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AJ33"/>
+      <c r="AK33"/>
+    </row>
+    <row r="34" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+    </row>
+    <row r="35" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+    </row>
+    <row r="36" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+    </row>
+    <row r="37" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+    </row>
+    <row r="38" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9EA430-F799-4BF0-8C78-87D528A8AA5B}">
   <dimension ref="A2:AK36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH31" sqref="AH31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
basic working - no config screens
</commit_message>
<xml_diff>
--- a/kbd_layout.xlsx
+++ b/kbd_layout.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradyumna\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50E9A1E-B02D-455B-BC0F-E0DFDFCE8FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564B2AA6-6191-4D71-B89A-0A31C06C6AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="1275" windowWidth="25245" windowHeight="16545" xr2:uid="{335468D2-36C8-4DD8-8A44-AE5A18BFA141}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{335468D2-36C8-4DD8-8A44-AE5A18BFA141}"/>
   </bookViews>
   <sheets>
-    <sheet name="manuform 6x7" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="2.0" sheetId="4" r:id="rId1"/>
+    <sheet name="manuform 6x7" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="187">
   <si>
     <t>* 8</t>
   </si>
@@ -579,6 +573,21 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                             </t>
+  </si>
+  <si>
+    <t>Mouse L</t>
+  </si>
+  <si>
+    <t>Mouse R</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>L Moon</t>
+  </si>
+  <si>
+    <t>R Moon</t>
   </si>
 </sst>
 </file>
@@ -620,7 +629,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -660,6 +669,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC3399"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -919,7 +952,7 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,6 +1069,57 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,8 +1128,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFCC3399"/>
+      <color rgb="FFEAB8D9"/>
       <color rgb="FF09B3D5"/>
-      <color rgb="FFEAB8D9"/>
       <color rgb="FFF99FE8"/>
     </mruColors>
   </colors>
@@ -1061,6 +1147,145 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Circle: Hollow 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29581499-689D-43BA-B320-A0EBCEF43A04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8096250" y="1228725"/>
+          <a:ext cx="209550" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="donut">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Circle: Hollow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD3D5E3-70BF-46B9-823E-1DBF74C7B27D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6686550" y="1228725"/>
+          <a:ext cx="209550" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="donut">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1266,7 +1491,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6501,11 +6726,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC6952D-12D4-41C7-BA70-FE890F76783D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6133C7D-C594-42C0-8C24-15093119726F}">
   <dimension ref="A2:AK38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6513,7 +6738,7 @@
     <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -6602,148 +6827,148 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" s="49" t="s">
+      <c r="H3" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="O3" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="49" t="s">
+      <c r="P3" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="49" t="s">
+      <c r="Q3" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="R3" s="53" t="s">
+      <c r="R3" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="53" t="s">
+      <c r="S3" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="53" t="s">
+      <c r="T3" s="70" t="s">
         <v>60</v>
       </c>
       <c r="V3" s="1">
         <v>0</v>
       </c>
-      <c r="W3" s="49" t="s">
+      <c r="W3" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="49" t="s">
+      <c r="X3" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="Y3" s="49" t="s">
+      <c r="Y3" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="Z3" s="49" t="s">
+      <c r="Z3" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="AA3" s="49" t="s">
+      <c r="AA3" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="49" t="s">
+      <c r="AB3" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="AC3" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD3" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE3" s="49" t="s">
+      <c r="AC3" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE3" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="49" t="s">
+      <c r="AF3" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="AG3" s="49" t="s">
+      <c r="AG3" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="AH3" s="49" t="s">
+      <c r="AH3" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="AI3" s="49" t="s">
+      <c r="AI3" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="AJ3" s="49" t="s">
+      <c r="AJ3" s="63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="N4" s="49" t="s">
-        <v>155</v>
-      </c>
-      <c r="O4" s="10" t="s">
+      <c r="H4" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="N4" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="73" t="s">
         <v>3</v>
       </c>
       <c r="V4" s="1">
         <v>1</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="W4" s="71" t="s">
         <v>43</v>
       </c>
       <c r="X4" s="13" t="s">
@@ -6761,11 +6986,11 @@
       <c r="AB4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AC4" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD4" s="49" t="s">
-        <v>155</v>
+      <c r="AC4" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD4" s="64" t="s">
+        <v>73</v>
       </c>
       <c r="AE4" s="13" t="s">
         <v>5</v>
@@ -6782,15 +7007,15 @@
       <c r="AI4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="AJ4" s="13" t="s">
+      <c r="AJ4" s="71" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="72" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -6808,11 +7033,11 @@
       <c r="G5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="N5" s="49" t="s">
-        <v>81</v>
+      <c r="H5" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="64" t="s">
+        <v>183</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>16</v>
@@ -6829,13 +7054,13 @@
       <c r="S5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="T5" s="71" t="s">
         <v>21</v>
       </c>
       <c r="V5" s="1">
         <v>2</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="72" t="s">
         <v>61</v>
       </c>
       <c r="X5" s="10" t="s">
@@ -6853,11 +7078,11 @@
       <c r="AB5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AC5" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD5" s="49" t="s">
-        <v>81</v>
+      <c r="AC5" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD5" s="64" t="s">
+        <v>183</v>
       </c>
       <c r="AE5" s="10" t="s">
         <v>16</v>
@@ -6874,15 +7099,15 @@
       <c r="AI5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AJ5" s="3" t="s">
+      <c r="AJ5" s="71" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="71" t="s">
         <v>85</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -6894,22 +7119,22 @@
       <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="63" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>88</v>
+      <c r="H6" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="64" t="s">
+        <v>182</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="63" t="s">
         <v>27</v>
       </c>
       <c r="Q6" s="10" t="s">
@@ -6921,13 +7146,13 @@
       <c r="S6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="72" t="s">
         <v>32</v>
       </c>
       <c r="V6" s="1">
         <v>3</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="71" t="s">
         <v>85</v>
       </c>
       <c r="X6" s="10" t="s">
@@ -6939,22 +7164,22 @@
       <c r="Z6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AA6" s="10" t="s">
+      <c r="AA6" s="63" t="s">
         <v>25</v>
       </c>
       <c r="AB6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AC6" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD6" s="33" t="s">
-        <v>88</v>
+      <c r="AC6" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD6" s="64" t="s">
+        <v>182</v>
       </c>
       <c r="AE6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AF6" s="10" t="s">
+      <c r="AF6" s="63" t="s">
         <v>27</v>
       </c>
       <c r="AG6" s="10" t="s">
@@ -6966,15 +7191,15 @@
       <c r="AI6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" s="71" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="72" t="s">
         <v>156</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -7007,13 +7232,13 @@
       <c r="S7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="T7" s="5" t="s">
-        <v>44</v>
+      <c r="T7" s="72" t="s">
+        <v>156</v>
       </c>
       <c r="V7" s="1">
         <v>4</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="72" t="s">
         <v>156</v>
       </c>
       <c r="X7" s="10" t="s">
@@ -7031,8 +7256,12 @@
       <c r="AB7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AC7"/>
-      <c r="AD7"/>
+      <c r="AC7" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD7" s="63" t="s">
+        <v>65</v>
+      </c>
       <c r="AE7" s="10" t="s">
         <v>38</v>
       </c>
@@ -7048,24 +7277,20 @@
       <c r="AI7" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AJ7" s="72" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="66" t="s">
         <v>46</v>
       </c>
       <c r="Q8" s="13" t="s">
@@ -7074,182 +7299,156 @@
       <c r="R8" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="S8"/>
+      <c r="T8"/>
       <c r="V8" s="1">
         <v>5</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="W8" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="X8" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y8" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="X8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="Z8" s="2" t="s">
+      <c r="Z8" s="64" t="s">
         <v>158</v>
       </c>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
-      <c r="AE8"/>
-      <c r="AF8"/>
+      <c r="AA8" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB8" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC8" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD8" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE8" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF8" s="63" t="s">
+        <v>63</v>
+      </c>
       <c r="AG8" s="13" t="s">
         <v>170</v>
       </c>
       <c r="AH8" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="AI8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ8" s="2" t="s">
-        <v>72</v>
+      <c r="AI8" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ8" s="63" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="F9" s="49" t="s">
+    <row r="9" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="I9" s="63" t="s">
         <v>68</v>
       </c>
       <c r="K9"/>
-      <c r="M9" s="49" t="s">
+      <c r="M9" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="49" t="s">
+      <c r="N9" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="49" t="s">
+      <c r="O9" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="P9" s="49" t="s">
+      <c r="P9" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="V9" s="1">
-        <v>6</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
       <c r="AC9"/>
       <c r="AD9"/>
-      <c r="AE9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+    </row>
+    <row r="10" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="AJ9" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="I10" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="M10" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="N10" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
     </row>
-    <row r="10" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H10" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="M10" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="N10" s="49" t="s">
-        <v>67</v>
-      </c>
+    <row r="11" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
+      <c r="AC11"/>
+      <c r="AD11"/>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
+      <c r="AK11"/>
     </row>
-    <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="V11" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="W11" s="1">
-        <v>0</v>
-      </c>
-      <c r="X11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>4</v>
-      </c>
-      <c r="AB11" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC11" s="1">
-        <v>6</v>
-      </c>
-      <c r="AD11" s="1">
-        <v>7</v>
-      </c>
-      <c r="AE11" s="1">
-        <v>8</v>
-      </c>
-      <c r="AF11" s="1">
-        <v>9</v>
-      </c>
-      <c r="AG11" s="1">
-        <v>10</v>
-      </c>
-      <c r="AH11" s="1">
-        <v>11</v>
-      </c>
-      <c r="AI11" s="1">
-        <v>12</v>
-      </c>
-      <c r="AJ11" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -7263,74 +7462,32 @@
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
-      <c r="N12" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="O12" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="P12" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q12" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="R12" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="S12" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="T12" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="V12" s="1">
-        <v>0</v>
-      </c>
-      <c r="W12" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="X12" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y12" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z12" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA12" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB12" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC12" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD12" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE12" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF12" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG12" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH12" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI12" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ12" s="49" t="s">
-        <v>60</v>
-      </c>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AK12"/>
     </row>
-    <row r="13" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -7344,523 +7501,384 @@
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="49" t="s">
-        <v>155</v>
-      </c>
-      <c r="O13" s="22" t="s">
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AK13"/>
+    </row>
+    <row r="14" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
         <v>5</v>
       </c>
-      <c r="P13" s="23">
+      <c r="H14" s="1">
+        <v>6</v>
+      </c>
+      <c r="N14" s="1">
         <v>7</v>
       </c>
-      <c r="Q13" s="24">
+      <c r="O14" s="1">
         <v>8</v>
       </c>
-      <c r="R13" s="43">
+      <c r="P14" s="1">
         <v>9</v>
       </c>
-      <c r="S13" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="T13" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="V13" s="1">
+      <c r="Q14" s="1">
+        <v>10</v>
+      </c>
+      <c r="R14" s="1">
+        <v>11</v>
+      </c>
+      <c r="S14" s="1">
+        <v>12</v>
+      </c>
+      <c r="T14" s="1">
+        <v>13</v>
+      </c>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+    </row>
+    <row r="15" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="N15" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="O15" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="P15" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q15" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="R15" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="S15" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="T15" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+    </row>
+    <row r="16" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>1</v>
       </c>
-      <c r="W13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="X13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC13" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD13" s="49" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF13" s="23">
-        <v>7</v>
-      </c>
-      <c r="AG13" s="24">
-        <v>8</v>
-      </c>
-      <c r="AH13" s="43">
-        <v>9</v>
-      </c>
-      <c r="AI13" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ13" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="P14" s="26">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="27">
-        <v>5</v>
-      </c>
-      <c r="R14" s="27">
-        <v>6</v>
-      </c>
-      <c r="S14" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="T14" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="V14" s="1">
-        <v>2</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC14" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD14" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF14" s="26">
-        <v>4</v>
-      </c>
-      <c r="AG14" s="27">
-        <v>5</v>
-      </c>
-      <c r="AH14" s="27">
-        <v>6</v>
-      </c>
-      <c r="AI14" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="27">
-        <v>2</v>
-      </c>
-      <c r="R15" s="27">
-        <v>3</v>
-      </c>
-      <c r="S15" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="V15" s="1">
-        <v>3</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="X15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC15" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD15" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF15" s="26">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="27">
-        <v>2</v>
-      </c>
-      <c r="AH15" s="27">
-        <v>3</v>
-      </c>
-      <c r="AI15" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="O16" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="P16" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q16" s="47">
-        <v>0</v>
-      </c>
-      <c r="R16" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="S16" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="V16" s="1">
-        <v>4</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="X16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB16" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="B16" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="64"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="62"/>
+      <c r="T16" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
       <c r="AC16"/>
       <c r="AD16"/>
-      <c r="AE16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF16" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG16" s="47">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI16" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ16" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
     </row>
     <row r="17" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="Q17" s="42" t="s">
-        <v>170</v>
-      </c>
-      <c r="R17" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="S17" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V17" s="1">
-        <v>5</v>
-      </c>
-      <c r="W17" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="Z17" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
       <c r="AA17"/>
       <c r="AB17"/>
       <c r="AC17"/>
       <c r="AD17"/>
       <c r="AE17"/>
       <c r="AF17"/>
-      <c r="AG17" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH17" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="AI17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ17" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
     </row>
     <row r="18" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="V18" s="1">
-        <v>6</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="64"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
       <c r="AC18"/>
       <c r="AD18"/>
-      <c r="AE18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ18" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
     </row>
     <row r="19" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="72" t="s">
+        <v>142</v>
+      </c>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
     </row>
     <row r="20" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
+      <c r="D20" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q20" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="R20" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="S20"/>
+      <c r="T20"/>
     </row>
     <row r="21" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
+      <c r="F21" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="63" t="s">
+        <v>123</v>
+      </c>
       <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
+      <c r="M21" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="N21" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="O21" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="P21" s="63" t="s">
+        <v>106</v>
+      </c>
       <c r="U21"/>
       <c r="V21"/>
       <c r="W21"/>
       <c r="X21"/>
     </row>
     <row r="22" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
+      <c r="H22" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="M22" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="N22" s="63" t="s">
+        <v>108</v>
+      </c>
       <c r="U22"/>
       <c r="V22"/>
       <c r="W22"/>
       <c r="X22"/>
     </row>
     <row r="23" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
@@ -8328,10 +8346,1837 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC6952D-12D4-41C7-BA70-FE890F76783D}">
+  <dimension ref="A2:AK38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1">
+        <v>12</v>
+      </c>
+      <c r="S2" s="1">
+        <v>13</v>
+      </c>
+      <c r="T2" s="1">
+        <v>14</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>12</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z3" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB3" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD3" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE3" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG3" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH3" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ3" s="49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="N4" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD4" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V5" s="1">
+        <v>2</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC5" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD5" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" s="1">
+        <v>3</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD6" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="1">
+        <v>4</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="1">
+        <v>5</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH8" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9"/>
+      <c r="M9" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1">
+        <v>6</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V11" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>11</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>12</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="P12" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q12" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="R12" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="S12" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="T12" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+      <c r="W12" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="X12" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y12" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z12" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA12" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB12" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC12" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD12" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE12" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF12" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG12" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH12" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI12" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ12" s="49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="23">
+        <v>7</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>8</v>
+      </c>
+      <c r="R13" s="43">
+        <v>9</v>
+      </c>
+      <c r="S13" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="T13" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13" s="1">
+        <v>1</v>
+      </c>
+      <c r="W13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="X13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC13" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD13" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF13" s="23">
+        <v>7</v>
+      </c>
+      <c r="AG13" s="24">
+        <v>8</v>
+      </c>
+      <c r="AH13" s="43">
+        <v>9</v>
+      </c>
+      <c r="AI13" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ13" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="26">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="27">
+        <v>5</v>
+      </c>
+      <c r="R14" s="27">
+        <v>6</v>
+      </c>
+      <c r="S14" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="T14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="V14" s="1">
+        <v>2</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC14" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD14" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF14" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="27">
+        <v>5</v>
+      </c>
+      <c r="AH14" s="27">
+        <v>6</v>
+      </c>
+      <c r="AI14" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>2</v>
+      </c>
+      <c r="R15" s="27">
+        <v>3</v>
+      </c>
+      <c r="S15" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V15" s="1">
+        <v>3</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="X15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC15" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD15" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF15" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="27">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="27">
+        <v>3</v>
+      </c>
+      <c r="AI15" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="O16" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="P16" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q16" s="47">
+        <v>0</v>
+      </c>
+      <c r="R16" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="S16" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" s="1">
+        <v>4</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="X16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF16" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG16" s="47">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI16" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="Q17" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="R17" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="S17" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V17" s="1">
+        <v>5</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH17" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="V18" s="1">
+        <v>6</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+    </row>
+    <row r="22" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+    </row>
+    <row r="23" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="AC23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+    </row>
+    <row r="24" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+    </row>
+    <row r="25" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+    </row>
+    <row r="26" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
+      <c r="AJ26"/>
+    </row>
+    <row r="27" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+    </row>
+    <row r="28" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+    </row>
+    <row r="29" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="AF29"/>
+      <c r="AG29"/>
+      <c r="AH29"/>
+      <c r="AI29"/>
+      <c r="AJ29"/>
+      <c r="AK29"/>
+    </row>
+    <row r="30" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="AF30"/>
+      <c r="AG30"/>
+      <c r="AH30"/>
+      <c r="AI30"/>
+      <c r="AJ30"/>
+      <c r="AK30"/>
+    </row>
+    <row r="31" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
+      <c r="AH31"/>
+      <c r="AI31"/>
+      <c r="AJ31"/>
+      <c r="AK31"/>
+    </row>
+    <row r="32" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+    </row>
+    <row r="33" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AJ33"/>
+      <c r="AK33"/>
+    </row>
+    <row r="34" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+    </row>
+    <row r="35" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+    </row>
+    <row r="36" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+    </row>
+    <row r="37" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+    </row>
+    <row r="38" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9EA430-F799-4BF0-8C78-87D528A8AA5B}">
   <dimension ref="A2:AK36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="AH31" sqref="AH31"/>
     </sheetView>
   </sheetViews>

</xml_diff>